<commit_message>
Continuação da documentação e melhorias
</commit_message>
<xml_diff>
--- a/Backlog AnimalFinder.xlsx
+++ b/Backlog AnimalFinder.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Animal Finder - Backlog</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Página principal dono (filtro animais pertencentes ao dono) (**)</t>
   </si>
   <si>
-    <t>Index animals - exibir foto (página principal allowed action) (****)</t>
-  </si>
-  <si>
     <t>Função Encontrei - com cadastro de encontrador - alterar status para comunicado</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>Criar a documentação do aplicativo</t>
   </si>
   <si>
-    <t>Documentação do aplicativo(**)</t>
-  </si>
-  <si>
     <t>Edit animal perdido (*)</t>
   </si>
   <si>
@@ -148,6 +142,18 @@
   </si>
   <si>
     <t>Subir para produção (****) (****)</t>
+  </si>
+  <si>
+    <t>Documentação do aplicativo(***)</t>
+  </si>
+  <si>
+    <t>Correção de Issues e melhorias</t>
+  </si>
+  <si>
+    <t>Correção de Issues e melhorias(****)</t>
+  </si>
+  <si>
+    <t>Index animals - exibir foto (página principal) (****)</t>
   </si>
 </sst>
 </file>
@@ -544,11 +550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:C11"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,8 +602,8 @@
       <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -610,8 +616,8 @@
       <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -663,7 +669,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -674,10 +680,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -685,7 +691,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -696,10 +702,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C12" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -707,20 +713,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="6">
         <v>8</v>
       </c>
-      <c r="C13" s="6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="5">
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5">
         <v>13</v>
       </c>
     </row>
@@ -731,11 +748,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -757,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -767,7 +784,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -777,10 +794,10 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -790,7 +807,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -800,14 +817,14 @@
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -821,7 +838,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -835,14 +852,14 @@
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -856,46 +873,48 @@
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="5"/>
       <c r="B16" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="B19" s="6"/>
       <c r="C19" s="1"/>
     </row>
@@ -1013,6 +1032,11 @@
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
API consulta animais perdidos
</commit_message>
<xml_diff>
--- a/Backlog AnimalFinder.xlsx
+++ b/Backlog AnimalFinder.xlsx
@@ -93,9 +93,6 @@
     <t>Botão encontrei - link para cadastro anjo e ao gravar alterar status para "Comunicado"(**)</t>
   </si>
   <si>
-    <t>API para uso externo com resposta json (****)</t>
-  </si>
-  <si>
     <t>" * " equivalem a dificuldade e provavel tempo gasto na implementação</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Index animals - exibir foto (página principal) (****)</t>
+  </si>
+  <si>
+    <t>API para uso externo com resposta json (**)</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -691,31 +691,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="6">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="6">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="6">
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1">
         <v>3</v>
       </c>
     </row>
@@ -724,7 +724,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="6">
         <v>8</v>
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5">
         <v>13</v>
@@ -752,7 +752,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -774,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -784,7 +784,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -794,10 +794,10 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -807,7 +807,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -817,14 +817,14 @@
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -838,7 +838,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -852,14 +852,14 @@
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -880,40 +880,40 @@
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="1"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="A17" s="5"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="6"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="1"/>

</xml_diff>